<commit_message>
M3 QA Cord #296 - Implements Cord Test Data #256   - Implements Cord Production #5     - Implements Export COA2
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA2.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA2.xlsx
@@ -598,7 +598,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -877,6 +877,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 2" xfId="5"/>
@@ -1287,7 +1288,7 @@
   <dimension ref="A1:FT79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -3132,6 +3133,7 @@
       <c r="A17" s="49" t="s">
         <v>34</v>
       </c>
+      <c r="B17" s="108"/>
       <c r="C17" s="50"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>

</xml_diff>